<commit_message>
various cleanups: Fix issues in tests; fix test data in library-example; allow complete maven build outside IDE including Kotlin and Surefire; fix some test class names; translate some German test names to English; disable various tests in 'architecture-tests' because of intentional violations (for demonstration purposes)
</commit_message>
<xml_diff>
--- a/library-example/src/test/resources/testdata/statistics/Movies.xlsx
+++ b/library-example/src/test/resources/testdata/statistics/Movies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mell/repos/schulung-vuwp/30_uebungen/36_Grosse-Uebung/library_Aufgabe/src/test/resources/testdata/statistics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\static-code-analysis-archunit\library-example\src\test\resources\testdata\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AE0248-5163-2740-87CF-04354EA9EFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB624C8F-C22D-4761-8464-662B649E4CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="3200" windowWidth="30820" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2565" yWindow="-120" windowWidth="26355" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>DVD</t>
   </si>
   <si>
-    <t>BLUERAY</t>
-  </si>
-  <si>
     <t>Spring: Von 0 auf 100 bis zum Frühling</t>
   </si>
   <si>
@@ -43,6 +40,9 @@
   </si>
   <si>
     <t>Grails: Wie Sie Ihren Gral finden</t>
+  </si>
+  <si>
+    <t>BLURAY</t>
   </si>
 </sst>
 </file>
@@ -82,7 +82,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -362,16 +362,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,28 +379,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>